<commit_message>
Actualización de los datos
</commit_message>
<xml_diff>
--- a/data/lab_instrumentos/raw/Lista de problemas LAB 1.xlsx
+++ b/data/lab_instrumentos/raw/Lista de problemas LAB 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uandresbelloedu-my.sharepoint.com/personal/c_moralesquiroz1_uandresbello_edu/Documents/Seremia MZ Austral_2021 comp/Laboratorio de instrumentos/Análisis de resultados LABs/datosMZaustral/data/lab_instrumentos/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3159521A-E465-4A99-AB28-D5FEF1ED297E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CD9E97A-8963-48CE-89FA-3BFC64BC4994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1755" yWindow="1185" windowWidth="24690" windowHeight="14355" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2349" uniqueCount="637">
   <si>
     <r>
       <rPr>
@@ -251,7 +251,7 @@
     <t>No hay claustro/cuerpo academico en las regiones debido a los requisitos actuales</t>
   </si>
   <si>
-    <t>insuficiente cantidad de investigadores Macrozona-Austral para docencia programas-postgrado</t>
+    <t>insuficiente investigadores Macrozona-Austral para docencia programas-postgrado</t>
   </si>
   <si>
     <t>Sistema de incentivos hacia individualización y en contra de cooperación (CNA, ANID).</t>
@@ -517,7 +517,7 @@
     <t>No estan pensados para suplir la realidad regional</t>
   </si>
   <si>
-    <t>No estan pensados para suplir la realidad de Macrozona-Austral</t>
+    <t xml:space="preserve"> No estan pensados para suplir la realidad de Macrozona-Austral</t>
   </si>
   <si>
     <t>bajo acceso equipamiento cientifico envio de muestras a otros lugares</t>
@@ -547,7 +547,7 @@
     <t>No esta claramente estipulado en las bases</t>
   </si>
   <si>
-    <t>No esta claramente estipulado en las bases-instrumento</t>
+    <t xml:space="preserve"> No esta claramente estipulado en las bases-instrumento</t>
   </si>
   <si>
     <t>Precarizacion del investigad@r y su linea de investigacion</t>
@@ -651,7 +651,7 @@
     <t>No existe otro instrumento/programa que de continuidad al proyecto para realizar mantención/reparación/calibración de equipamiento cientifico</t>
   </si>
   <si>
-    <t>No existe otro instrumento que de continuidad a proyectos para realizar mantención reparación calibración de equipamiento</t>
+    <t xml:space="preserve"> No existe otro instrumento que de continuidad a proyectos para realizar mantención reparación calibración de equipamiento</t>
   </si>
   <si>
     <t>Las instituciones (universidades) no tienen recursos para hacer mantenciones o comprar repuestos</t>
@@ -697,7 +697,7 @@
     <t>No se permite contratar a estudiantes chilenos que no estén vinculados a universidades nacionales</t>
   </si>
   <si>
-    <t>No se permite contratar a estudiantes-pregrado estudiantes-postgrado chilenos que no estén vinculados a universidades chilenas</t>
+    <t xml:space="preserve"> No se permite contratar a estudiantes-pregrado estudiantes-postgrado chilenos que no estén vinculados a universidades chilenas</t>
   </si>
   <si>
     <t xml:space="preserve">Pocos estudiantes disponibles de pre y postgrado </t>
@@ -881,7 +881,7 @@
     <t>Es insuficiente el monto asignado por bases</t>
   </si>
   <si>
-    <t>Es insuficiente el monto asignado por bases-instrumento</t>
+    <t>insuficiente montos asignados por bases-instrumento</t>
   </si>
   <si>
     <t>disminuye la colaboración internacional</t>
@@ -947,7 +947,7 @@
     <t>Decisiones a distancia y sin apelación tomadas por administrativos que desconocen la realidad economica y aislamiento austral</t>
   </si>
   <si>
-    <t>Decisiones a distancia y sin apelación tomadas por administrativos que desconocen la realidad-economica y aislamiento-austral</t>
+    <t>Decisiones a distancia y sin apelación tomadas por administrativos no-reconoce la realidad-economica y aislamiento-austral</t>
   </si>
   <si>
     <t>Recursos alcanzan para menos items que en otras regiones, competencia injusta</t>
@@ -986,7 +986,7 @@
     <t>No hay personas que participen y cooperen en los proyectos</t>
   </si>
   <si>
-    <t>insuficientes universidades en Macrozona-Austral con pocos estudiantes-pregrado estudiantes-postgrado profesionales-investigación</t>
+    <t>insuficiente universidades en Macrozona-Austral con pocos estudiantes-pregrado estudiantes-postgrado profesionales-investigación</t>
   </si>
   <si>
     <t>Base de datos CNED 
@@ -1065,7 +1065,7 @@
     <t>No hay claustro/cuerpo académico en las regiones debido a los requisitos actuales</t>
   </si>
   <si>
-    <t>No hay claustro/cuerpo académico en Macrozona-Austral debido a los requisitos actuales</t>
+    <t xml:space="preserve"> No hay claustro/cuerpo académico en Macrozona-Austral debido a los requisitos actuales</t>
   </si>
   <si>
     <t>Sistema de incentivos hacia individualización y en contra de cooperación (CNA, ANID)</t>
@@ -1137,7 +1137,7 @@
     <t>Solo una Universidad Estatal en ambas regiones con pocos alumnos</t>
   </si>
   <si>
-    <t>insuficientes universidades en Macrozona-Austral con pocos estudiantes-pregrado</t>
+    <t>insuficiente universidades en Macrozona-Austral con pocos estudiantes-pregrado</t>
   </si>
   <si>
     <t>la duración de 24 meses de los proyectos FONDEF no es suficiente</t>
@@ -1287,7 +1287,7 @@
     <t>Que en la región existen pocos profesionales de apoyo en el área científica y para incluirlos en los proyectos deben ser atraídos desde otras regiones o rubros</t>
   </si>
   <si>
-    <t>Insuficiente profesionales-investigación en Macrozona-Austral y para incluirlos en los proyectos deben ser atraídos desde otras regiones o rubros</t>
+    <t>insuficiente profesionales-investigación en Macrozona-Austral y para incluirlos en los proyectos deben ser atraídos desde otras regiones o rubros</t>
   </si>
   <si>
     <t>Los incentivos son deficientes para justificar el traslado de doctores y postdoctorados a zonas extremas</t>
@@ -1299,7 +1299,7 @@
     <t>que tenemos pocas instituciones empleadoras de profesionales con esas características</t>
   </si>
   <si>
-    <t>que tenemos insuficientes instituciones empleadoras de profesionales-de-la-investigación con esas características</t>
+    <t>insuficiente instituciones empleadoras de profesionales-de-la-investigación con esas características</t>
   </si>
   <si>
     <t>Proyectos con menos investigadores, menos capacidad de trabajo y menor productividad, asociada a la cantidad de profesionales especialistas en los temas de la investigación</t>
@@ -1312,7 +1312,7 @@
     <t>No hay doctores ni postdoctorados en zonas extremas</t>
   </si>
   <si>
-    <t>insuficiente doctores y postdoctorados en Macrozona-Austral</t>
+    <t>insuficiente profesionales-investigación en Macrozona-Austral</t>
   </si>
   <si>
     <t>Los profesionales se retiran en medio de los proyectos</t>
@@ -1438,7 +1438,7 @@
     <t>No esta establecido en las bases de ANID</t>
   </si>
   <si>
-    <t>No esta establecido en las bases-instrumento de ANID</t>
+    <t xml:space="preserve"> No esta establecido en las bases-instrumento de ANID</t>
   </si>
   <si>
     <t>Investigador@ principal cumple todas las funciones de un equipo de trabajo y no puede ampliar linea de investigación y/o contrata con su sueldo a alguien</t>
@@ -1550,6 +1550,9 @@
   </si>
   <si>
     <t>cambios/restricciones de ANID desconocidos</t>
+  </si>
+  <si>
+    <t>cambios restricciones de ANID desconocidos</t>
   </si>
   <si>
     <t>Limita y perjudicada las redes internacionales que han servido para cerrar brechas regionales a traves de la colaboracion con capital humano (escaso en la region), y la disponibilidad de equipamiento e infraestructura ausente en la region</t>
@@ -2913,12 +2916,16 @@
   <autoFilter ref="A1:L154" xr:uid="{FE410A01-264B-43B2-8193-30E6CE711D62}">
     <filterColumn colId="7">
       <filters>
-        <filter val="El instrumento no tiene diferencias entre instalacion de equipamiento en laboratorios, terreno, zonas de alto riesgo y zonas extremas con alto aislamiento"/>
-        <filter val="instrumento sin-diferenciación entre instalacion de equipamiento en laboratorios, terreno, zonas de alto riesgo y zonas extremas con alto aislamiento"/>
-        <filter val="instrumento sin-diferenciación entre instalación de equipamiento en laboratorios, terreno, zonas de alto riesgo y zonas extremas con alto aislamiento"/>
-        <filter val="insuficiente recursos universidades para adquirir equipamiento de manera total o en cofinanciamiento para los nuevos proyectos"/>
-        <filter val="para equipamiento costos mantención mayores, costo calibración mayores, costos para técnicos mayores y costos reparaciones mayores"/>
-        <filter val="Solicitan como indicador más personas que usen el equipamiento dentro de la institución"/>
+        <filter val="insuficientes apoyo-administrativo para los proyectos en universidades"/>
+        <filter val="insuficientes doctores y postdoctorados en Macrozona-Austral"/>
+        <filter val="insuficientes instituciones empleadoras de profesionales-de-la-investigación con esas características"/>
+        <filter val="insuficientes investigadores Macrozona-Austral para docencia programas-postgrado"/>
+        <filter val="insuficientes montos asignados por bases-instrumento"/>
+        <filter val="Insuficientes profesionales-investigación en Macrozona-Austral y para incluirlos en los proyectos deben ser atraídos desde otras regiones o rubros"/>
+        <filter val="insuficientes programas-postgrado programa de doctorado en Macrozona-Austral"/>
+        <filter val="insuficientes recursos universidades para adquirir equipamiento-científico de manera total o en cofinanciamiento para los nuevos proyectos"/>
+        <filter val="insuficientes universidades en Macrozona-Austral con pocos estudiantes-pregrado"/>
+        <filter val="insuficientes universidades en Macrozona-Austral con pocos estudiantes-pregrado estudiantes-postgrado profesionales-investigación"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -4554,7 +4561,7 @@
       </c>
       <c r="L38" s="69"/>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+    <row r="39" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A39" s="14" t="s">
         <v>59</v>
       </c>
@@ -5252,7 +5259,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="58" spans="1:12" ht="15.75" customHeight="1">
       <c r="A58" s="3" t="s">
         <v>59</v>
       </c>
@@ -5560,7 +5567,7 @@
       </c>
       <c r="L66" s="63"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" customHeight="1">
+    <row r="67" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A67" s="20" t="s">
         <v>59</v>
       </c>
@@ -5596,7 +5603,7 @@
       </c>
       <c r="L67" s="67"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" customHeight="1">
+    <row r="68" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A68" s="20" t="s">
         <v>59</v>
       </c>
@@ -5632,7 +5639,7 @@
       </c>
       <c r="L68" s="67"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" customHeight="1">
+    <row r="69" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A69" s="20" t="s">
         <v>59</v>
       </c>
@@ -5668,7 +5675,7 @@
       </c>
       <c r="L69" s="67"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" customHeight="1">
+    <row r="70" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A70" s="20" t="s">
         <v>59</v>
       </c>
@@ -5704,7 +5711,7 @@
       </c>
       <c r="L70" s="67"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" customHeight="1">
+    <row r="71" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A71" s="20" t="s">
         <v>59</v>
       </c>
@@ -5740,7 +5747,7 @@
       </c>
       <c r="L71" s="67"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" customHeight="1">
+    <row r="72" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A72" s="20" t="s">
         <v>59</v>
       </c>
@@ -5776,7 +5783,7 @@
       </c>
       <c r="L72" s="67"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" customHeight="1">
+    <row r="73" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A73" s="20" t="s">
         <v>59</v>
       </c>
@@ -5878,7 +5885,7 @@
       <c r="K75" s="13"/>
       <c r="L75" s="63"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="76" spans="1:12" ht="15.75" customHeight="1">
       <c r="A76" s="3" t="s">
         <v>59</v>
       </c>
@@ -5916,7 +5923,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="77" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="77" spans="1:12" ht="15.75" customHeight="1">
       <c r="A77" s="3" t="s">
         <v>59</v>
       </c>
@@ -5954,7 +5961,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="78" spans="1:12" ht="15.75" customHeight="1">
       <c r="A78" s="3" t="s">
         <v>59</v>
       </c>
@@ -6618,7 +6625,7 @@
       </c>
       <c r="L96" s="55"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="97" spans="1:12" ht="15.75" customHeight="1">
       <c r="A97" s="16" t="s">
         <v>13</v>
       </c>
@@ -6804,7 +6811,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="102" spans="1:12" ht="15.75" customHeight="1">
+    <row r="102" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A102" s="12" t="s">
         <v>59</v>
       </c>
@@ -6870,7 +6877,7 @@
       <c r="K103" s="13"/>
       <c r="L103" s="63"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" customHeight="1">
+    <row r="104" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A104" s="12" t="s">
         <v>59</v>
       </c>
@@ -6938,7 +6945,7 @@
       </c>
       <c r="L105" s="63"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="106" spans="1:12" ht="15.75" customHeight="1">
       <c r="A106" s="16" t="s">
         <v>13</v>
       </c>
@@ -6974,7 +6981,7 @@
       </c>
       <c r="L106" s="57"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="107" spans="1:12" ht="15.75" customHeight="1">
       <c r="A107" s="16" t="s">
         <v>13</v>
       </c>
@@ -7152,7 +7159,7 @@
       </c>
       <c r="L111" s="63"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" customHeight="1">
+    <row r="112" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A112" s="12" t="s">
         <v>59</v>
       </c>
@@ -7188,7 +7195,7 @@
       </c>
       <c r="L112" s="63"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" customHeight="1">
+    <row r="113" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A113" s="12" t="s">
         <v>59</v>
       </c>
@@ -7404,7 +7411,7 @@
       </c>
       <c r="L118" s="63"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="119" spans="1:12" ht="15.75" customHeight="1">
       <c r="A119" s="3" t="s">
         <v>13</v>
       </c>
@@ -7442,7 +7449,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="120" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="120" spans="1:12" ht="15.75" customHeight="1">
       <c r="A120" s="3" t="s">
         <v>29</v>
       </c>
@@ -7480,7 +7487,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="121" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="121" spans="1:12" ht="15.75" customHeight="1">
       <c r="A121" s="3" t="s">
         <v>29</v>
       </c>
@@ -7858,7 +7865,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="131" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="131" spans="1:12" ht="15.75" customHeight="1">
       <c r="A131" s="9" t="s">
         <v>29</v>
       </c>
@@ -7894,7 +7901,7 @@
       </c>
       <c r="L131" s="59"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="132" spans="1:12" ht="15.75" customHeight="1">
       <c r="A132" s="9" t="s">
         <v>29</v>
       </c>
@@ -7930,7 +7937,7 @@
       </c>
       <c r="L132" s="59"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="133" spans="1:12" ht="15.75" customHeight="1">
       <c r="A133" s="9" t="s">
         <v>29</v>
       </c>
@@ -8222,7 +8229,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="141" spans="1:12" ht="15.75" customHeight="1">
+    <row r="141" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A141" s="16" t="s">
         <v>59</v>
       </c>
@@ -8258,7 +8265,7 @@
       </c>
       <c r="L141" s="57"/>
     </row>
-    <row r="142" spans="1:12" ht="15.75" customHeight="1">
+    <row r="142" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A142" s="16" t="s">
         <v>59</v>
       </c>
@@ -8294,7 +8301,7 @@
       </c>
       <c r="L142" s="57"/>
     </row>
-    <row r="143" spans="1:12" ht="15.75" customHeight="1">
+    <row r="143" spans="1:12" ht="15.75" hidden="1" customHeight="1">
       <c r="A143" s="16" t="s">
         <v>59</v>
       </c>
@@ -8436,7 +8443,7 @@
       </c>
       <c r="L146" s="63"/>
     </row>
-    <row r="147" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="147" spans="1:12" ht="15.75" customHeight="1">
       <c r="A147" s="3" t="s">
         <v>59</v>
       </c>
@@ -8472,7 +8479,7 @@
       </c>
       <c r="L147" s="3"/>
     </row>
-    <row r="148" spans="1:12" ht="15.75" hidden="1" customHeight="1">
+    <row r="148" spans="1:12" ht="15.75" customHeight="1">
       <c r="A148" s="3" t="s">
         <v>13</v>
       </c>
@@ -8627,13 +8634,13 @@
         <v>453</v>
       </c>
       <c r="H152" s="64" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="I152" s="64" t="s">
         <v>20</v>
       </c>
       <c r="J152" s="64" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K152" s="15">
         <v>1</v>
@@ -8648,34 +8655,34 @@
         <v>38</v>
       </c>
       <c r="C153" s="50" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="D153" s="50" t="s">
         <v>32</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F153" s="50" t="s">
         <v>32</v>
       </c>
       <c r="G153" s="50" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="H153" s="50" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="I153" s="3" t="s">
         <v>35</v>
       </c>
       <c r="J153" s="50" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="K153" s="4">
         <v>0</v>
       </c>
       <c r="L153" s="49" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="154" spans="1:12" ht="15.75" hidden="1" customHeight="1">
@@ -8686,28 +8693,28 @@
         <v>38</v>
       </c>
       <c r="C154" s="50" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D154" s="50" t="s">
         <v>95</v>
       </c>
       <c r="E154" s="50" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="F154" s="3" t="s">
         <v>95</v>
       </c>
       <c r="G154" s="50" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="H154" s="50" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="I154" s="3" t="s">
         <v>35</v>
       </c>
       <c r="J154" s="50" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="K154" s="4">
         <v>0</v>
@@ -8771,58 +8778,58 @@
         <v>1</v>
       </c>
       <c r="B1" s="78" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C1" s="78" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="78" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="E1" s="78" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="12.75">
       <c r="A2" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="12.75">
       <c r="A3" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B3" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>378</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12.75">
       <c r="A4" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B4" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>170</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E4" s="49" t="s">
         <v>218</v>
@@ -8830,86 +8837,86 @@
     </row>
     <row r="5" spans="1:5" ht="12.75">
       <c r="A5" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B5" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C5" s="49" t="s">
         <v>388</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="12.75">
       <c r="A6" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C6" s="49" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="12.75">
       <c r="A7" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C7" s="49" t="s">
         <v>406</v>
       </c>
       <c r="D7" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="12.75">
       <c r="A8" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C8" s="49" t="s">
         <v>406</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="12.75">
       <c r="A9" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C9" s="49" t="s">
         <v>121</v>
       </c>
       <c r="D9" s="49" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="12.75">
       <c r="A10" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C10" s="49" t="s">
         <v>201</v>
       </c>
       <c r="D10" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E10" s="49" t="s">
         <v>218</v>
@@ -8917,27 +8924,27 @@
     </row>
     <row r="11" spans="1:5" ht="12.75">
       <c r="A11" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C11" s="49" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12.75">
       <c r="A12" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C12" s="49" t="s">
         <v>170</v>
@@ -8948,24 +8955,24 @@
     </row>
     <row r="13" spans="1:5" ht="12.75">
       <c r="A13" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C13" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D13" s="49" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12.75">
       <c r="A14" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C14" s="49" t="s">
         <v>211</v>
@@ -8977,16 +8984,16 @@
     </row>
     <row r="15" spans="1:5" ht="12.75">
       <c r="A15" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B15" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C15" s="49" t="s">
         <v>265</v>
       </c>
       <c r="D15" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E15" s="49" t="s">
         <v>218</v>
@@ -8994,24 +9001,24 @@
     </row>
     <row r="16" spans="1:5" ht="12.75">
       <c r="A16" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C16" s="49" t="s">
         <v>419</v>
       </c>
       <c r="D16" s="49" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="12.75">
       <c r="A17" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B17" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C17" s="49" t="s">
         <v>170</v>
@@ -9022,89 +9029,89 @@
     </row>
     <row r="18" spans="1:5" ht="12.75">
       <c r="A18" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C18" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D18" s="71" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="12.75">
       <c r="A19" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D19" s="71" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="12.75">
       <c r="A20" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C20" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D20" s="71" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="12.75">
       <c r="A21" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C21" s="49" t="s">
         <v>406</v>
       </c>
       <c r="D21" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="12.75">
       <c r="A22" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C22" s="49" t="s">
         <v>201</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="12.75">
       <c r="A23" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B23" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C23" s="49" t="s">
         <v>265</v>
       </c>
       <c r="D23" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E23" s="49" t="s">
         <v>218</v>
@@ -9112,10 +9119,10 @@
     </row>
     <row r="24" spans="1:5" ht="12.75">
       <c r="A24" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B24" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C24" s="49" t="s">
         <v>201</v>
@@ -9126,30 +9133,30 @@
     </row>
     <row r="25" spans="1:5" ht="12.75">
       <c r="A25" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B25" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C25" s="49" t="s">
         <v>201</v>
       </c>
       <c r="D25" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="12.75">
       <c r="A26" s="49" t="s">
+        <v>475</v>
+      </c>
+      <c r="B26" s="49" t="s">
+        <v>472</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>497</v>
+      </c>
+      <c r="D26" s="49" t="s">
         <v>474</v>
-      </c>
-      <c r="B26" s="49" t="s">
-        <v>471</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>496</v>
-      </c>
-      <c r="D26" s="49" t="s">
-        <v>473</v>
       </c>
       <c r="E26" s="49" t="s">
         <v>218</v>
@@ -9157,30 +9164,30 @@
     </row>
     <row r="27" spans="1:5" ht="12.75">
       <c r="A27" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B27" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C27" s="49" t="s">
         <v>265</v>
       </c>
       <c r="D27" s="49" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="12.75">
       <c r="A28" s="49" t="s">
+        <v>475</v>
+      </c>
+      <c r="B28" s="49" t="s">
+        <v>472</v>
+      </c>
+      <c r="C28" s="49" t="s">
+        <v>499</v>
+      </c>
+      <c r="D28" s="49" t="s">
         <v>474</v>
-      </c>
-      <c r="B28" s="49" t="s">
-        <v>471</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>498</v>
-      </c>
-      <c r="D28" s="49" t="s">
-        <v>473</v>
       </c>
       <c r="E28" s="49" t="s">
         <v>218</v>
@@ -9188,10 +9195,10 @@
     </row>
     <row r="29" spans="1:5" ht="12.75">
       <c r="A29" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B29" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C29" s="49" t="s">
         <v>265</v>
@@ -9202,593 +9209,593 @@
     </row>
     <row r="30" spans="1:5" ht="12.75">
       <c r="A30" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B30" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C30" s="49" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D30" s="49" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="12.75">
       <c r="A31" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B31" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C31" s="49" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="D31" s="49" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="12.75">
       <c r="A32" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B32" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C32" s="49" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="D32" s="49" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="12.75">
       <c r="A33" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B33" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C33" s="49" t="s">
         <v>362</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="E33" s="49" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="12.75">
       <c r="A34" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B34" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C34" s="49" t="s">
         <v>378</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="12.75">
       <c r="A35" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C35" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="12.75">
       <c r="A36" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C36" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="12.75">
       <c r="A37" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B37" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C37" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D37" s="49" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="12.75">
       <c r="A38" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B38" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C38" s="49" t="s">
         <v>367</v>
       </c>
       <c r="D38" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="12.75">
       <c r="A39" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B39" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C39" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D39" s="49" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="12.75">
       <c r="A40" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B40" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C40" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D40" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E40" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="12.75">
       <c r="A41" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B41" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C41" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D41" s="49" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="12.75">
       <c r="A42" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B42" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C42" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D42" s="49" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="12.75">
       <c r="A43" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B43" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C43" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D43" s="49" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="12.75">
       <c r="A44" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B44" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C44" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D44" s="49" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="12.75">
       <c r="A45" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C45" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D45" s="49" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="12.75">
       <c r="A46" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C46" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D46" s="49" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="12.75">
       <c r="A47" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B47" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C47" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D47" s="49" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="12.75">
       <c r="A48" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B48" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C48" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D48" s="49" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="12.75">
       <c r="A49" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B49" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C49" s="49" t="s">
         <v>51</v>
       </c>
       <c r="D49" s="49" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="12.75">
       <c r="A50" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B50" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C50" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D50" s="49" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="12.75">
       <c r="A51" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B51" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C51" s="49" t="s">
         <v>150</v>
       </c>
       <c r="D51" s="49" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="12.75">
       <c r="A52" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B52" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C52" s="49" t="s">
         <v>419</v>
       </c>
       <c r="D52" s="49" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="12.75">
       <c r="A53" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B53" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C53" s="49" t="s">
         <v>150</v>
       </c>
       <c r="D53" s="49" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="12.75">
       <c r="A54" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B54" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C54" s="49" t="s">
         <v>150</v>
       </c>
       <c r="D54" s="49" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="12.75">
       <c r="A55" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B55" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C55" s="49" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D55" s="49" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="E55" s="49" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="12.75">
       <c r="A56" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B56" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C56" s="49" t="s">
         <v>150</v>
       </c>
       <c r="D56" s="49" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="12.75">
       <c r="A57" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B57" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C57" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D57" s="49" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="12.75">
       <c r="A58" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B58" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C58" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D58" s="49" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="12.75">
       <c r="A59" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B59" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C59" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D59" s="49" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="12.75">
       <c r="A60" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B60" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C60" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D60" s="49" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="12.75">
       <c r="A61" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B61" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C61" s="49" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D61" s="49" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="12.75">
       <c r="A62" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B62" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C62" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D62" s="49" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="12.75">
       <c r="A63" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B63" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C63" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D63" s="49" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="12.75">
       <c r="A64" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B64" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C64" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D64" s="49" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="12.75">
       <c r="A65" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B65" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C65" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D65" s="49" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="12.75">
       <c r="A66" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B66" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C66" s="49" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D66" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="12.75">
       <c r="A67" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B67" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C67" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D67" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="12.75">
       <c r="A68" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B68" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C68" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D68" s="49" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="12.75">
       <c r="A69" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B69" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C69" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D69" s="49" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="12.75">
       <c r="A70" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B70" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C70" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D70" s="49" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="12.75">
       <c r="A71" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B71" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C71" s="49" t="s">
         <v>367</v>
@@ -9799,480 +9806,480 @@
     </row>
     <row r="72" spans="1:5" ht="12.75">
       <c r="A72" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B72" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C72" s="49" t="s">
         <v>367</v>
       </c>
       <c r="D72" s="49" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="12.75">
       <c r="A73" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B73" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C73" s="49" t="s">
         <v>388</v>
       </c>
       <c r="D73" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E73" s="49" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="12.75">
       <c r="A74" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B74" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C74" s="49" t="s">
         <v>367</v>
       </c>
       <c r="D74" s="49" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="12.75">
       <c r="A75" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B75" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C75" s="49" t="s">
         <v>367</v>
       </c>
       <c r="D75" s="49" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="12.75">
       <c r="A76" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B76" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C76" s="49" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D76" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="12.75">
       <c r="A77" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B77" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C77" s="49" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D77" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="78" spans="1:5" ht="12.75">
       <c r="A78" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B78" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C78" s="49" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D78" s="49" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="79" spans="1:5" ht="12.75">
       <c r="A79" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B79" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C79" s="49" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D79" s="49" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="80" spans="1:5" ht="12.75">
       <c r="A80" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B80" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C80" s="49" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D80" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="81" spans="1:5" ht="12.75">
       <c r="A81" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B81" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C81" s="49" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D81" s="49" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="12.75">
       <c r="A82" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B82" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C82" s="49" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D82" s="49" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="83" spans="1:5" ht="12.75">
       <c r="A83" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B83" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C83" s="49" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="D83" s="49" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="84" spans="1:5" ht="12.75">
       <c r="A84" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B84" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C84" s="49" t="s">
         <v>219</v>
       </c>
       <c r="D84" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="12.75">
       <c r="A85" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B85" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C85" s="49" t="s">
         <v>287</v>
       </c>
       <c r="D85" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="12.75">
       <c r="A86" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B86" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C86" s="49" t="s">
         <v>388</v>
       </c>
       <c r="D86" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="12.75">
       <c r="A87" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B87" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C87" s="49" t="s">
         <v>388</v>
       </c>
       <c r="D87" s="49" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="12.75">
       <c r="A88" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B88" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C88" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D88" s="49" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="12.75">
       <c r="A89" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B89" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C89" s="49" t="s">
         <v>452</v>
       </c>
       <c r="D89" s="49" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E89" s="49" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="12.75">
       <c r="A90" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B90" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C90" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D90" s="49" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="12.75">
       <c r="A91" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B91" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C91" s="49" t="s">
         <v>424</v>
       </c>
       <c r="D91" s="49" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="12.75">
       <c r="A92" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B92" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C92" s="49" t="s">
         <v>194</v>
       </c>
       <c r="D92" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="12.75">
       <c r="A93" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B93" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C93" s="49" t="s">
         <v>170</v>
       </c>
       <c r="D93" s="49" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="12.75">
       <c r="A94" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B94" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C94" s="49" t="s">
         <v>121</v>
       </c>
       <c r="D94" s="49" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E94" s="49"/>
     </row>
     <row r="95" spans="1:5" ht="12.75">
       <c r="A95" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B95" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C95" s="49" t="s">
         <v>211</v>
       </c>
       <c r="D95" s="49" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="E95" s="49" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="12.75">
       <c r="A96" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B96" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C96" s="49" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D96" s="49" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E96" s="49" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="12.75">
       <c r="A97" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B97" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C97" s="49" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D97" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="98" spans="1:5" ht="12.75">
       <c r="A98" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B98" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C98" s="49" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D98" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="99" spans="1:5" ht="12.75">
       <c r="A99" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B99" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C99" s="49" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D99" s="49" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="12.75">
       <c r="A100" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B100" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C100" s="49" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D100" s="49" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E100" s="70" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="12.75">
       <c r="A101" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B101" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C101" s="49" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="D101" s="49" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="102" spans="1:5" ht="12.75">
       <c r="A102" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B102" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C102" s="49" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D102" s="49" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="12.75">
       <c r="A103" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B103" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C103" s="49" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D103" s="49" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="12.75">
       <c r="A104" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B104" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C104" s="49" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D104" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E104" s="49" t="s">
         <v>218</v>
@@ -10280,13 +10287,13 @@
     </row>
     <row r="105" spans="1:5" ht="12.75">
       <c r="A105" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B105" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C105" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D105" s="71" t="s">
         <v>106</v>
@@ -10294,44 +10301,44 @@
     </row>
     <row r="106" spans="1:5" ht="12.75">
       <c r="A106" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B106" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C106" s="49" t="s">
         <v>338</v>
       </c>
       <c r="D106" s="49" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="107" spans="1:5" ht="12.75">
       <c r="A107" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B107" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C107" s="49" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D107" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="12.75">
       <c r="A108" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B108" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C108" s="49" t="s">
         <v>287</v>
       </c>
       <c r="D108" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E108" s="49" t="s">
         <v>218</v>
@@ -10339,150 +10346,150 @@
     </row>
     <row r="109" spans="1:5" ht="12.75">
       <c r="A109" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B109" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C109" s="49" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D109" s="49" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="12.75">
       <c r="A110" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B110" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C110" s="49" t="s">
         <v>116</v>
       </c>
       <c r="D110" s="49" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="111" spans="1:5" ht="12.75">
       <c r="A111" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B111" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C111" s="49" t="s">
         <v>116</v>
       </c>
       <c r="D111" s="49" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="12.75">
       <c r="A112" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B112" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C112" s="49" t="s">
         <v>116</v>
       </c>
       <c r="D112" s="49" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="12.75">
       <c r="A113" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B113" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C113" s="49" t="s">
         <v>116</v>
       </c>
       <c r="D113" s="49" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="114" spans="1:5" ht="12.75">
       <c r="A114" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B114" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C114" s="49" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D114" s="49" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="115" spans="1:5" ht="12.75">
       <c r="A115" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B115" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C115" s="49" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D115" s="49" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="12.75">
       <c r="A116" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B116" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C116" s="49" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D116" s="49" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="12.75">
       <c r="A117" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B117" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C117" s="49" t="s">
+        <v>575</v>
+      </c>
+      <c r="D117" s="49" t="s">
         <v>574</v>
-      </c>
-      <c r="D117" s="49" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="12.75">
       <c r="A118" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B118" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C118" s="49" t="s">
         <v>302</v>
       </c>
       <c r="D118" s="49" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="119" spans="1:5" ht="12.75">
       <c r="A119" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B119" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C119" s="49" t="s">
         <v>302</v>
@@ -10493,13 +10500,13 @@
     </row>
     <row r="120" spans="1:5" ht="12.75">
       <c r="A120" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B120" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C120" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D120" s="49" t="s">
         <v>106</v>
@@ -10507,13 +10514,13 @@
     </row>
     <row r="121" spans="1:5" ht="12.75">
       <c r="A121" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B121" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C121" s="49" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D121" s="49" t="s">
         <v>106</v>
@@ -10521,30 +10528,30 @@
     </row>
     <row r="122" spans="1:5" ht="12.75">
       <c r="A122" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B122" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C122" s="49" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D122" s="49" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="123" spans="1:5" ht="12.75">
       <c r="A123" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B123" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C123" s="49" t="s">
         <v>194</v>
       </c>
       <c r="D123" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E123" s="49" t="s">
         <v>218</v>
@@ -10552,162 +10559,162 @@
     </row>
     <row r="124" spans="1:5" ht="12.75">
       <c r="A124" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B124" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C124" s="49" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D124" s="49" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="125" spans="1:5" ht="12.75">
       <c r="A125" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B125" s="49" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C125" s="49" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="D125" s="49" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="126" spans="1:5" ht="12.75">
       <c r="A126" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B126" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C126" s="49" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="D126" s="49" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="127" spans="1:5" ht="12.75">
       <c r="A127" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B127" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C127" s="49" t="s">
         <v>219</v>
       </c>
       <c r="D127" s="49" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="E127" s="49" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="128" spans="1:5" ht="12.75">
       <c r="A128" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B128" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C128" s="49" t="s">
         <v>219</v>
       </c>
       <c r="D128" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="129" spans="1:5" ht="12.75">
       <c r="A129" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B129" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C129" s="49" t="s">
         <v>219</v>
       </c>
       <c r="D129" s="49" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="130" spans="1:5" ht="12.75">
       <c r="A130" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B130" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C130" s="49" t="s">
         <v>219</v>
       </c>
       <c r="D130" s="49" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="12.75">
       <c r="A131" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B131" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C131" s="49" t="s">
         <v>287</v>
       </c>
       <c r="D131" s="49" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="132" spans="1:5" ht="12.75">
       <c r="A132" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B132" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C132" s="49" t="s">
         <v>287</v>
       </c>
       <c r="D132" s="49" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="133" spans="1:5" ht="12.75">
       <c r="A133" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B133" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C133" s="49" t="s">
         <v>219</v>
       </c>
       <c r="D133" s="49" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="E133" s="49" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="12.75">
       <c r="A134" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B134" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C134" s="49" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D134" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E134" s="49" t="s">
         <v>218</v>
@@ -10715,184 +10722,184 @@
     </row>
     <row r="135" spans="1:5" ht="12.75">
       <c r="A135" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B135" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C135" s="49" t="s">
         <v>188</v>
       </c>
       <c r="D135" s="49" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="136" spans="1:5" ht="12.75">
       <c r="A136" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B136" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C136" s="49" t="s">
         <v>188</v>
       </c>
       <c r="D136" s="49" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="137" spans="1:5" ht="12.75">
       <c r="A137" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B137" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C137" s="49" t="s">
         <v>188</v>
       </c>
       <c r="D137" s="49" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="12.75">
       <c r="A138" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B138" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C138" s="49" t="s">
         <v>188</v>
       </c>
       <c r="D138" s="49" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="12.75">
       <c r="A139" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B139" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C139" s="49" t="s">
         <v>61</v>
       </c>
       <c r="D139" s="49" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="12.75">
       <c r="A140" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B140" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C140" s="49" t="s">
         <v>452</v>
       </c>
       <c r="D140" s="49" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="141" spans="1:5" ht="12.75">
       <c r="A141" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B141" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C141" s="49" t="s">
         <v>452</v>
       </c>
       <c r="D141" s="49" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="12.75">
       <c r="A142" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B142" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C142" s="49" t="s">
         <v>150</v>
       </c>
       <c r="D142" s="49" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="12.75">
       <c r="A143" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B143" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C143" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D143" s="49" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="144" spans="1:5" ht="12.75">
       <c r="A144" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B144" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C144" s="49" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D144" s="49" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="145" spans="1:5" ht="12.75">
       <c r="A145" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B145" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C145" s="49" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="D145" s="49" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="12.75">
       <c r="A146" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B146" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C146" s="49" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="D146" s="49" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="12.75">
       <c r="A147" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B147" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C147" s="49" t="s">
         <v>362</v>
       </c>
       <c r="D147" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E147" s="49" t="s">
         <v>218</v>
@@ -10900,10 +10907,10 @@
     </row>
     <row r="148" spans="1:5" ht="12.75">
       <c r="A148" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B148" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C148" s="49" t="s">
         <v>194</v>
@@ -10914,100 +10921,100 @@
     </row>
     <row r="149" spans="1:5" ht="12.75">
       <c r="A149" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B149" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C149" s="49" t="s">
         <v>170</v>
       </c>
       <c r="D149" s="49" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="12.75">
       <c r="A150" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B150" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C150" s="49" t="s">
         <v>194</v>
       </c>
       <c r="D150" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="151" spans="1:5" ht="12.75">
       <c r="A151" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B151" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C151" s="49" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D151" s="49" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="152" spans="1:5" ht="12.75">
       <c r="A152" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B152" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C152" s="49" t="s">
         <v>201</v>
       </c>
       <c r="D152" s="49" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="153" spans="1:5" ht="12.75">
       <c r="A153" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B153" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C153" s="49" t="s">
         <v>211</v>
       </c>
       <c r="D153" s="49" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="154" spans="1:5" ht="12.75">
       <c r="A154" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B154" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C154" s="49" t="s">
         <v>211</v>
       </c>
       <c r="D154" s="49" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="155" spans="1:5" ht="12.75">
       <c r="A155" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B155" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C155" s="49" t="s">
         <v>51</v>
       </c>
       <c r="D155" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E155" s="49" t="s">
         <v>218</v>
@@ -11015,27 +11022,27 @@
     </row>
     <row r="156" spans="1:5" ht="12.75">
       <c r="A156" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B156" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C156" s="49" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="D156" s="49" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="12.75">
       <c r="A157" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B157" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C157" s="49" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D157" s="49" t="s">
         <v>100</v>
@@ -11043,86 +11050,86 @@
     </row>
     <row r="158" spans="1:5" ht="12.75">
       <c r="A158" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B158" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C158" s="49" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D158" s="49" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="159" spans="1:5" ht="12.75">
       <c r="A159" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B159" s="49" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C159" s="49" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="D159" s="49" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="12.75">
       <c r="A160" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B160" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C160" s="49" t="s">
         <v>205</v>
       </c>
       <c r="D160" s="49" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="12.75">
       <c r="A161" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B161" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C161" s="49" t="s">
         <v>205</v>
       </c>
       <c r="D161" s="49" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="162" spans="1:5" ht="12.75">
       <c r="A162" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B162" s="49" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C162" s="49" t="s">
         <v>150</v>
       </c>
       <c r="D162" s="49" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="163" spans="1:5" ht="12.75">
       <c r="A163" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B163" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C163" s="49" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D163" s="49" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E163" s="49" t="s">
         <v>218</v>
@@ -11130,10 +11137,10 @@
     </row>
     <row r="164" spans="1:5" ht="12.75">
       <c r="A164" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B164" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C164" s="49" t="s">
         <v>362</v>
@@ -11144,44 +11151,44 @@
     </row>
     <row r="165" spans="1:5" ht="12.75">
       <c r="A165" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B165" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C165" s="49" t="s">
         <v>362</v>
       </c>
       <c r="D165" s="49" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="12.75">
       <c r="A166" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B166" s="49" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C166" s="49" t="s">
         <v>302</v>
       </c>
       <c r="D166" s="49" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="12.75">
       <c r="A167" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B167" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C167" s="49" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="D167" s="49" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="E167" s="49" t="s">
         <v>218</v>
@@ -11189,10 +11196,10 @@
     </row>
     <row r="168" spans="1:5" ht="12.75">
       <c r="A168" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B168" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C168" s="49" t="s">
         <v>51</v>
@@ -11203,58 +11210,58 @@
     </row>
     <row r="169" spans="1:5" ht="12.75">
       <c r="A169" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B169" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C169" s="49" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D169" s="49" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="170" spans="1:5" ht="12.75">
       <c r="A170" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B170" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C170" s="49" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D170" s="49" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="171" spans="1:5" ht="15.75" customHeight="1">
       <c r="A171" s="49" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B171" s="49" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C171" s="49" t="s">
         <v>121</v>
       </c>
       <c r="D171" s="49" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="15.75" customHeight="1">
       <c r="A172" s="49" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="B172" s="49" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C172" s="49" t="s">
         <v>419</v>
       </c>
       <c r="D172" s="49" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="E172" s="49" t="s">
         <v>218</v>
@@ -11262,13 +11269,13 @@
     </row>
     <row r="173" spans="1:5" ht="15.75" customHeight="1">
       <c r="A173" s="49" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B173" s="49" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C173" s="49" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="D173" s="49" t="s">
         <v>100</v>
@@ -11301,64 +11308,64 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="B1" s="81" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C1" s="82"/>
       <c r="D1" s="81" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="E1" s="82"/>
       <c r="F1" s="81" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="G1" s="82"/>
       <c r="H1" s="81" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="I1" s="82"/>
       <c r="J1" s="81" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="K1" s="82"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="C2" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="D2" s="25" t="s">
-        <v>616</v>
-      </c>
       <c r="E2" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="F2" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="F2" s="25" t="s">
-        <v>616</v>
-      </c>
       <c r="G2" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="H2" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>616</v>
-      </c>
       <c r="I2" s="26" t="s">
+        <v>618</v>
+      </c>
+      <c r="J2" s="25" t="s">
         <v>617</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>616</v>
-      </c>
       <c r="K2" s="26" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="27" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="B3" s="28">
         <v>35620</v>
@@ -11393,7 +11400,7 @@
     </row>
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="27" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B4" s="28">
         <v>7316</v>
@@ -11428,7 +11435,7 @@
     </row>
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="27" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B5" s="28">
         <v>8945</v>
@@ -11463,7 +11470,7 @@
     </row>
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="B6" s="34">
         <v>129</v>
@@ -11498,7 +11505,7 @@
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B7" s="28">
         <v>11267</v>
@@ -11533,7 +11540,7 @@
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B8" s="28">
         <v>1322</v>
@@ -11568,7 +11575,7 @@
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="27" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B9" s="28">
         <v>2035</v>
@@ -11603,7 +11610,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="27" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B10" s="34">
         <v>464</v>
@@ -11638,7 +11645,7 @@
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="27" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="B11" s="28">
         <v>1115</v>
@@ -11673,7 +11680,7 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="27" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B12" s="28">
         <v>3136</v>
@@ -11708,7 +11715,7 @@
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B13" s="28">
         <v>3491</v>
@@ -11743,7 +11750,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="36" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="B14" s="37">
         <v>4586</v>
@@ -11778,7 +11785,7 @@
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="36" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="B15" s="37">
         <v>3265</v>
@@ -11813,7 +11820,7 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B16" s="34">
         <v>989</v>
@@ -11848,7 +11855,7 @@
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="27" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="B17" s="34">
         <v>243</v>
@@ -11883,7 +11890,7 @@
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="27" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="B18" s="34">
         <v>0</v>
@@ -11918,7 +11925,7 @@
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B19" s="34">
         <v>0</v>
@@ -11953,7 +11960,7 @@
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="45" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B20" s="46">
         <v>83923</v>

</xml_diff>